<commit_message>
Filled in the last benchmark row and added some decimals to the power columns.
</commit_message>
<xml_diff>
--- a/Docs/BenchmarksVitis.xlsx
+++ b/Docs/BenchmarksVitis.xlsx
@@ -1,26 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\aux_c\repositories\c-sharp\Hastlayer-SDK-Vitis\Docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repositories\c-sharp\Hastlayer-SDK-Vitis\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{3F2517FE-92CB-4370-9BA8-5FFD42E6D74C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38DDF9C8-FFC6-4BC1-B71D-539E3087D0E5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="330" windowWidth="29040" windowHeight="15990"/>
+    <workbookView xWindow="-120" yWindow="330" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Benchmarks" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="21">
   <si>
     <t>Device</t>
   </si>
@@ -83,19 +94,17 @@
   </si>
   <si>
     <t>Alveo U50</t>
-  </si>
-  <si>
-    <t xml:space="preserve">      </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="3">
-    <numFmt numFmtId="166" formatCode="0\ &quot;ms&quot;"/>
-    <numFmt numFmtId="167" formatCode="0\ &quot;Ws&quot;"/>
-    <numFmt numFmtId="168" formatCode="0\ &quot;W&quot;"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="4">
+    <numFmt numFmtId="164" formatCode="0\ &quot;ms&quot;"/>
+    <numFmt numFmtId="165" formatCode="0\ &quot;Ws&quot;"/>
+    <numFmt numFmtId="171" formatCode="0.00\ &quot;W&quot;"/>
+    <numFmt numFmtId="172" formatCode="0.00\ &quot;Ws&quot;"/>
   </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
@@ -574,13 +583,14 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -935,11 +945,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L17" sqref="A2:L17"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -954,7 +964,7 @@
     <col min="8" max="8" width="15.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="9.42578125" style="3" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="10.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.85546875" style="6" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="19.28515625" style="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -989,7 +999,7 @@
       <c r="J1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="K1" s="6" t="s">
         <v>10</v>
       </c>
       <c r="L1" s="5" t="s">
@@ -1030,7 +1040,7 @@
       <c r="J2" s="3">
         <v>65</v>
       </c>
-      <c r="K2" s="4">
+      <c r="K2" s="6">
         <f>L2*J2/1000</f>
         <v>1.5527849999999999</v>
       </c>
@@ -1072,7 +1082,7 @@
       <c r="J3" s="3">
         <v>5586</v>
       </c>
-      <c r="K3" s="4">
+      <c r="K3" s="6">
         <f t="shared" ref="K3:K17" si="3">L3*J3/1000</f>
         <v>133.44395399999999</v>
       </c>
@@ -1114,7 +1124,7 @@
       <c r="J4" s="3">
         <v>140</v>
       </c>
-      <c r="K4" s="4">
+      <c r="K4" s="6">
         <f t="shared" si="3"/>
         <v>2.1806399999999999</v>
       </c>
@@ -1156,7 +1166,7 @@
       <c r="J5" s="3">
         <v>67</v>
       </c>
-      <c r="K5" s="4">
+      <c r="K5" s="6">
         <f t="shared" si="3"/>
         <v>1.275345</v>
       </c>
@@ -1198,7 +1208,7 @@
       <c r="J6" s="3">
         <v>33</v>
       </c>
-      <c r="K6" s="4">
+      <c r="K6" s="6">
         <f t="shared" si="3"/>
         <v>0.83212800000000009</v>
       </c>
@@ -1240,7 +1250,7 @@
       <c r="J7" s="3">
         <v>5735</v>
       </c>
-      <c r="K7" s="4">
+      <c r="K7" s="6">
         <f t="shared" si="3"/>
         <v>144.61376000000001</v>
       </c>
@@ -1282,7 +1292,7 @@
       <c r="J8" s="3">
         <v>109</v>
       </c>
-      <c r="K8" s="4">
+      <c r="K8" s="6">
         <f t="shared" si="3"/>
         <v>1.7665630000000001</v>
       </c>
@@ -1324,7 +1334,7 @@
       <c r="J9" s="3">
         <v>42</v>
       </c>
-      <c r="K9" s="4">
+      <c r="K9" s="6">
         <f t="shared" si="3"/>
         <v>0.83542199999999989</v>
       </c>
@@ -1366,7 +1376,7 @@
       <c r="J10" s="3">
         <v>32</v>
       </c>
-      <c r="K10" s="4">
+      <c r="K10" s="6">
         <f t="shared" si="3"/>
         <v>0.73712</v>
       </c>
@@ -1408,7 +1418,7 @@
       <c r="J11" s="3">
         <v>494</v>
       </c>
-      <c r="K11" s="4">
+      <c r="K11" s="6">
         <f t="shared" si="3"/>
         <v>11.379290000000001</v>
       </c>
@@ -1450,7 +1460,7 @@
       <c r="J12" s="3">
         <v>111</v>
       </c>
-      <c r="K12" s="4">
+      <c r="K12" s="6">
         <f t="shared" si="3"/>
         <v>1.6636679999999999</v>
       </c>
@@ -1492,7 +1502,7 @@
       <c r="J13" s="3">
         <v>38</v>
       </c>
-      <c r="K13" s="4">
+      <c r="K13" s="6">
         <f t="shared" si="3"/>
         <v>0.66689999999999994</v>
       </c>
@@ -1534,7 +1544,7 @@
       <c r="J14" s="3">
         <v>33</v>
       </c>
-      <c r="K14" s="4">
+      <c r="K14" s="6">
         <f t="shared" si="3"/>
         <v>0.654918</v>
       </c>
@@ -1576,7 +1586,7 @@
       <c r="J15" s="3">
         <v>482</v>
       </c>
-      <c r="K15" s="4">
+      <c r="K15" s="6">
         <f t="shared" si="3"/>
         <v>9.5657720000000008</v>
       </c>
@@ -1595,9 +1605,9 @@
         <f t="shared" si="0"/>
         <v>2.5754716981132075</v>
       </c>
-      <c r="D16" s="2" t="e">
+      <c r="D16" s="2">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>26.534222027054735</v>
       </c>
       <c r="E16">
         <v>300</v>
@@ -1609,8 +1619,8 @@
         <f t="shared" si="2"/>
         <v>34.11</v>
       </c>
-      <c r="H16" s="1" t="s">
-        <v>21</v>
+      <c r="H16" s="1">
+        <v>0.16220000000000001</v>
       </c>
       <c r="I16" s="3">
         <v>104</v>
@@ -1618,9 +1628,12 @@
       <c r="J16" s="3">
         <v>106</v>
       </c>
-      <c r="K16" s="4">
+      <c r="K16" s="6">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1.2388219999999999</v>
+      </c>
+      <c r="L16" s="5">
+        <v>11.686999999999999</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
@@ -1657,7 +1670,7 @@
       <c r="J17" s="3">
         <v>44</v>
       </c>
-      <c r="K17" s="4">
+      <c r="K17" s="6">
         <f t="shared" si="3"/>
         <v>0.634876</v>
       </c>

</xml_diff>